<commit_message>
Anpassung Modul an API v2 für HW Rev. v3
</commit_message>
<xml_diff>
--- a/docs/go-eCharger Interface.xlsx
+++ b/docs/go-eCharger Interface.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d024440/Documents/PrivateGitHubs/GO-eCharger/go-eCharger/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d024440/Documents/PrivateGitHubs/GO-eCharger/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E883E62E-7819-1A4A-9562-6CCD2B969E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACA26D2-2C1F-4D4C-8C39-6F644DA5633F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36520" yWindow="2740" windowWidth="30700" windowHeight="22480" activeTab="1" xr2:uid="{7C6B8FB2-F957-6243-B808-C31D85E7D9C2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="446">
   <si>
     <t>IPS Bezeichnung</t>
   </si>
@@ -1990,9 +1990,6 @@
     <t>temperatureCurrentLimit (ampere)</t>
   </si>
   <si>
-    <t>frc muss zum Starten/Stoppen verwendet werden!</t>
-  </si>
-  <si>
     <t>Is the car allowed to charge at all now?
 Ist nur noch ein Status!</t>
   </si>
@@ -2077,6 +2074,12 @@
   <si>
     <t>Kann kombiniert gemacht werden
 z.B. acs=0&amp;lmo=3&amp;frc=0&amp;dwo=16000 (=Access Control = Open + default logic mode + frc = 0 (startet automatisch) + max. 16kWh laden)</t>
+  </si>
+  <si>
+    <t>frc muss zum Starten/Stoppen zw. für den Default-Mode gesetzt  verwendet werden!</t>
+  </si>
+  <si>
+    <t>v3 Charger müssen zusätzlich via frc in den "default mode" gesetzt werden</t>
   </si>
 </sst>
 </file>
@@ -2280,7 +2283,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2355,7 +2358,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4545,8 +4548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C077908E-DCE3-6949-B77F-58CCED76ABE2}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4630,7 +4633,7 @@
         <v>339</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>17</v>
@@ -4648,13 +4651,13 @@
         <v>231</v>
       </c>
       <c r="E5" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="38" t="s">
         <v>438</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4669,13 +4672,13 @@
         <v>231</v>
       </c>
       <c r="E6" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="G6" s="38" t="s">
         <v>438</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4690,13 +4693,13 @@
         <v>231</v>
       </c>
       <c r="E7" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="G7" s="38" t="s">
         <v>438</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4711,13 +4714,13 @@
         <v>231</v>
       </c>
       <c r="E8" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="G8" s="38" t="s">
         <v>438</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4732,13 +4735,13 @@
         <v>231</v>
       </c>
       <c r="E9" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="G9" s="38" t="s">
         <v>438</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4761,10 +4764,10 @@
         <v>404</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>427</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="31" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4868,7 +4871,7 @@
         <v>423</v>
       </c>
       <c r="H15" s="46" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4885,13 +4888,13 @@
         <v>372</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F16" s="37" t="s">
         <v>400</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -4968,6 +4971,9 @@
       <c r="G19" s="14" t="s">
         <v>383</v>
       </c>
+      <c r="H19" s="19" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
@@ -5272,7 +5278,7 @@
         <v>410</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D33" s="39" t="s">
         <v>377</v>
@@ -5281,13 +5287,13 @@
         <v>14</v>
       </c>
       <c r="F33" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="G33" s="14" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="37" t="s">
         <v>329</v>
       </c>
@@ -5310,23 +5316,23 @@
         <v>355</v>
       </c>
       <c r="H34" s="45" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="C35" s="14"/>
       <c r="D35" s="26"/>
       <c r="E35" s="37" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F35" s="37" t="s">
         <v>400</v>
       </c>
       <c r="G35" s="38" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H35" s="46" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -5361,13 +5367,13 @@
       <c r="C37" s="29"/>
       <c r="D37" s="30"/>
       <c r="E37" s="37" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F37" s="37" t="s">
         <v>400</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -5579,7 +5585,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="37" t="s">
         <v>13</v>
       </c>

</xml_diff>